<commit_message>
DDT bug finding is done.
</commit_message>
<xml_diff>
--- a/src/test/resources/Book2.xlsx
+++ b/src/test/resources/Book2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mohai\IdeaProjects\WebAutomationWithPOM\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ABCBCB8-5A3F-4CF4-A5C8-7425B485F927}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{377D7FFA-5A7D-4A14-898E-2E0ECF2133A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{4105F128-8E5C-49E9-8B4B-175C2A729B91}"/>
   </bookViews>
@@ -25,37 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="29">
-  <si>
-    <t>FirstName</t>
-  </si>
-  <si>
-    <t>LastName</t>
-  </si>
-  <si>
-    <t>Address</t>
-  </si>
-  <si>
-    <t>City</t>
-  </si>
-  <si>
-    <t>State</t>
-  </si>
-  <si>
-    <t>ZipCode</t>
-  </si>
-  <si>
-    <t>PhoneNumber</t>
-  </si>
-  <si>
-    <t>SSN</t>
-  </si>
-  <si>
-    <t>UserName</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="19">
   <si>
     <t>123-4560-789</t>
   </si>
@@ -78,24 +48,6 @@
     <t>123password</t>
   </si>
   <si>
-    <t>user30</t>
-  </si>
-  <si>
-    <t>user31</t>
-  </si>
-  <si>
-    <t>user32</t>
-  </si>
-  <si>
-    <t>user33</t>
-  </si>
-  <si>
-    <t>user34</t>
-  </si>
-  <si>
-    <t>user35</t>
-  </si>
-  <si>
     <t>nayeem01</t>
   </si>
   <si>
@@ -112,6 +64,24 @@
   </si>
   <si>
     <t>nayeem06</t>
+  </si>
+  <si>
+    <t>test01</t>
+  </si>
+  <si>
+    <t>test02</t>
+  </si>
+  <si>
+    <t>test03</t>
+  </si>
+  <si>
+    <t>test04</t>
+  </si>
+  <si>
+    <t>test05</t>
+  </si>
+  <si>
+    <t>test06</t>
   </si>
 </sst>
 </file>
@@ -469,10 +439,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B2B66F2-4407-49E4-98D3-1E0B6B1AD79E}">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -491,226 +461,194 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1">
+        <v>1234567890</v>
+      </c>
+      <c r="H1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" t="s">
         <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="F2" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="G2">
         <v>1234567890</v>
       </c>
       <c r="H2" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="I2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="J2" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="F3" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="G3">
         <v>1234567890</v>
       </c>
       <c r="H3" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="I3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="J3" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="F4" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="G4">
         <v>1234567890</v>
       </c>
       <c r="H4" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="I4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="J4" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="E5" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="F5" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="G5">
         <v>1234567890</v>
       </c>
       <c r="H5" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="I5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="J5" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="E6" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="F6" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="G6">
         <v>1234567890</v>
       </c>
       <c r="H6" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="I6" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="J6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C7" t="s">
-        <v>28</v>
-      </c>
-      <c r="D7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E7" t="s">
-        <v>28</v>
-      </c>
-      <c r="F7" t="s">
-        <v>28</v>
-      </c>
-      <c r="G7">
-        <v>1234567890</v>
-      </c>
-      <c r="H7" t="s">
-        <v>15</v>
-      </c>
-      <c r="I7" t="s">
-        <v>22</v>
-      </c>
-      <c r="J7" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>